<commit_message>
#72627 - Data Quality Report template issues fixed for datetime, decimal and alignment related. Unit test missing data issue fixed.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6672F026-80A9-47B4-8DD3-FA649FB2F0C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7849CB-C2A2-4028-8B49-F78889AE169B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ILR Data Quality Reports" sheetId="4" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>&amp;=Top10ProvidersWithInvalidLearners.Status</t>
   </si>
   <si>
-    <t>&amp;=Top10ProvidersWithInvalidLearners.LatestReturnPeriod</t>
-  </si>
-  <si>
     <t>&amp;=Top10ProvidersWithInvalidLearners.NoOfValidLearners</t>
   </si>
   <si>
@@ -160,12 +157,6 @@
     <t>&amp;=Top10ProvidersWithInvalidLearners.LatestFileName</t>
   </si>
   <si>
-    <t>&amp;=Top10ProvidersWithInvalidLearners.DateSubmitted</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=(G{r}/F{r})*100</t>
-  </si>
-  <si>
     <t>ILR Data Quality Reports - Rnn</t>
   </si>
   <si>
@@ -173,6 +164,15 @@
   </si>
   <si>
     <t>Latest File Submitted</t>
+  </si>
+  <si>
+    <t>&amp;=Top10ProvidersWithInvalidLearners.LatestReturn</t>
+  </si>
+  <si>
+    <t>&amp;=Top10ProvidersWithInvalidLearners.SubmittedDateTime</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=ROUND((G{r}/F{r})*100,2)</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -410,7 +410,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -459,9 +459,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -486,7 +483,15 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -916,23 +921,23 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="2"/>
-    <col min="2" max="2" width="30.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="45.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.53515625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.15234375" style="2"/>
+    <col min="4" max="4" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="45.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5703125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -945,7 +950,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>29</v>
       </c>
@@ -960,7 +965,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="2:16" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -973,7 +978,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:16" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
@@ -988,31 +993,31 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="2:16" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="26" t="s">
+    <row r="6" spans="2:16" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="20" t="s">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -1021,14 +1026,14 @@
       <c r="E7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="17.600000000000001" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1037,9 +1042,9 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:16" ht="16.3" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>11</v>
@@ -1054,11 +1059,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -1071,7 +1076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1087,107 +1092,107 @@
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="2:16" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="29" t="s">
+    <row r="13" spans="2:16" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="2:16" ht="13.3" x14ac:dyDescent="0.35">
-      <c r="B14" s="25" t="s">
+    <row r="14" spans="2:16" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D14" s="23"/>
+      <c r="E14" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="26.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31" t="s">
+    <row r="17" spans="2:10" ht="26.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-    </row>
-    <row r="18" spans="2:10" ht="26.6" x14ac:dyDescent="0.35">
-      <c r="B18" s="23" t="s">
+      <c r="C17" s="33"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="2:10" ht="27" x14ac:dyDescent="0.2">
+      <c r="B18" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="27" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="G19" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="H19" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>45</v>
+      <c r="J19" s="28" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#86735 - Data Quality Report bug fixed where multiple file detail records were read and template issue where it was displaying division errro is fixed and collection management package added into internal service and service projects.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7849CB-C2A2-4028-8B49-F78889AE169B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8B1910-E6C7-42FD-8D87-981C162275F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11010" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ILR Data Quality Reports" sheetId="4" r:id="rId1"/>
@@ -172,7 +172,7 @@
     <t>&amp;=Top10ProvidersWithInvalidLearners.SubmittedDateTime</t>
   </si>
   <si>
-    <t>&amp;=&amp;=ROUND((G{r}/F{r})*100,2)</t>
+    <t>&amp;=&amp;=IF((OR(G{r}=0, F{r}=0)), 0, ROUND((G{r}/F{r})*100,2))</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -489,10 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,6 +503,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -917,25 +917,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F22A55-F14A-458E-B18C-794EF0F5CA37}">
   <dimension ref="B2:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.15234375" style="2"/>
+    <col min="2" max="2" width="30.69140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="45.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="29.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="45.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.53515625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="8" t="s">
         <v>44</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="9" t="s">
         <v>29</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="14.6" x14ac:dyDescent="0.4">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -978,7 +978,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:16" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="2:16" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" ht="17.600000000000001" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1042,7 +1042,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:16" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>45</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" ht="24.9" x14ac:dyDescent="0.35">
       <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1092,15 +1092,15 @@
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="2:16" ht="21.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
+    <row r="13" spans="2:16" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="2:16" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" ht="13.3" x14ac:dyDescent="0.35">
       <c r="B14" s="24" t="s">
         <v>24</v>
       </c>
@@ -1112,23 +1112,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="26.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="32" t="s">
+    <row r="17" spans="2:10" ht="26.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
@@ -1137,7 +1137,7 @@
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
     </row>
-    <row r="18" spans="2:10" ht="27" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" ht="26.6" x14ac:dyDescent="0.35">
       <c r="B18" s="22" t="s">
         <v>24</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="26" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Update to templates, collection stats percentage and limit Top 10 Providers with Invalid Learners back to 10!
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8B1910-E6C7-42FD-8D87-981C162275F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{74FA48C7-3060-4DF3-AF16-125F6734E4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F24288A3-CBB9-4DCF-9AD8-63FF4936A758}"/>
   <bookViews>
-    <workbookView xWindow="-11010" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ILR Data Quality Reports" sheetId="4" r:id="rId1"/>
+    <sheet name="Data Quality" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,6 +49,9 @@
     <t>Top 20 Rule Violations</t>
   </si>
   <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
     <t>Providers</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Last File Submitted</t>
+  </si>
+  <si>
     <t>&amp;=ProviderWithoutValidLearnerInfo.Ukprn</t>
   </si>
   <si>
@@ -115,6 +121,9 @@
     <t>Report Run: &lt;Date &amp; Time&gt;</t>
   </si>
   <si>
+    <t>ILR Data Quality Report - Rnn</t>
+  </si>
+  <si>
     <t>Top 10 Providers with Invalid Learners</t>
   </si>
   <si>
@@ -157,22 +166,13 @@
     <t>&amp;=Top10ProvidersWithInvalidLearners.LatestFileName</t>
   </si>
   <si>
-    <t>ILR Data Quality Reports - Rnn</t>
-  </si>
-  <si>
-    <t>Rule  Name</t>
-  </si>
-  <si>
-    <t>Latest File Submitted</t>
-  </si>
-  <si>
     <t>&amp;=Top10ProvidersWithInvalidLearners.LatestReturn</t>
   </si>
   <si>
     <t>&amp;=Top10ProvidersWithInvalidLearners.SubmittedDateTime</t>
   </si>
   <si>
-    <t>&amp;=&amp;=IF((OR(G{r}=0, F{r}=0)), 0, ROUND((G{r}/F{r})*100,2))</t>
+    <t>&amp;=&amp;=(H{r}/(H{r}+G{r}))*100</t>
   </si>
 </sst>
 </file>
@@ -181,9 +181,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,6 +192,22 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -214,6 +230,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -221,86 +246,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="0"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,30 +295,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDA0DD"/>
-        <bgColor rgb="FFDDA0DD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90EE90"/>
-        <bgColor rgb="FF90EE90"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -391,121 +359,78 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD3D3D3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFD3D3D3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -917,289 +842,294 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F22A55-F14A-458E-B18C-794EF0F5CA37}">
   <dimension ref="B2:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="2"/>
-    <col min="2" max="2" width="30.69140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="45.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.69140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.53515625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.15234375" style="2"/>
+    <col min="1" max="1" width="9.1328125" style="3"/>
+    <col min="2" max="2" width="30.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.3984375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.06640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="22.265625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="2:16" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="2:16" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
+    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="2:16" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="2:16" ht="18" x14ac:dyDescent="0.4">
+      <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="2:16" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="18" x14ac:dyDescent="0.4">
+      <c r="B9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="17.600000000000001" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="2:16" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="24.9" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="2:16" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="30"/>
+    </row>
+    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="2:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="2:16" ht="13.3" x14ac:dyDescent="0.35">
-      <c r="B14" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="24" t="s">
+    <row r="14" spans="2:16" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24" t="s">
+      <c r="C14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="2:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B18" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B19" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="26.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-    </row>
-    <row r="18" spans="2:10" ht="26.6" x14ac:dyDescent="0.35">
-      <c r="B18" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J19" s="28" t="s">
+      <c r="K19" s="27" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Data Quality Report fixes
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{74FA48C7-3060-4DF3-AF16-125F6734E4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F24288A3-CBB9-4DCF-9AD8-63FF4936A758}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEA1747-166F-49C9-B853-ADB18EA6CB8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Quality" sheetId="4" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>No of Valid Learners</t>
   </si>
   <si>
-    <t>Pct Invalid Learners</t>
-  </si>
-  <si>
     <t>Last File Name</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>&amp;=&amp;=(H{r}/(H{r}+G{r}))*100</t>
+  </si>
+  <si>
+    <t>% Invalid Learners</t>
   </si>
 </sst>
 </file>
@@ -842,27 +842,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F22A55-F14A-458E-B18C-794EF0F5CA37}">
   <dimension ref="B2:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="3"/>
-    <col min="2" max="2" width="30.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.86328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.3984375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="50.06640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="22.265625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="3"/>
+    <col min="4" max="4" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50" style="3" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
@@ -877,7 +877,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
@@ -892,7 +892,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:16" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -905,7 +905,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:16" ht="18" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:16" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
@@ -940,7 +940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
@@ -960,7 +960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="18" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:16" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -986,7 +986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1019,7 +1019,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="14"/>
     </row>
-    <row r="13" spans="2:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>24</v>
       </c>
@@ -1027,7 +1027,7 @@
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="2:16" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
         <v>25</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="25" t="s">
         <v>33</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
     </row>
-    <row r="18" spans="2:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>25</v>
       </c>
@@ -1086,43 +1086,43 @@
         <v>36</v>
       </c>
       <c r="I18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="K18" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="K18" s="26" t="s">
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B19" s="22" t="s">
+      <c r="C19" s="28" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>42</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="27" t="s">
         <v>47</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#92943 correcting opening position within template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ILRDataQualityReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5B03E0-9916-4603-924E-78463F7A71F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8F51E7-7D7C-4975-A778-3A2C29C90B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Quality" sheetId="4" r:id="rId1"/>
@@ -426,13 +426,13 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -843,27 +843,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F22A55-F14A-458E-B18C-794EF0F5CA37}">
   <dimension ref="B2:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="3"/>
+    <col min="2" max="2" width="30.73046875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.3984375" style="3" customWidth="1"/>
     <col min="10" max="10" width="50" style="3" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="11" max="11" width="22.265625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -906,7 +906,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:16" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="18" x14ac:dyDescent="0.4">
       <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
@@ -921,7 +921,7 @@
       <c r="K5"/>
       <c r="L5"/>
     </row>
-    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
@@ -961,7 +961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" ht="18" x14ac:dyDescent="0.4">
       <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -987,7 +987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1020,7 +1020,7 @@
       <c r="O12" s="13"/>
       <c r="P12" s="14"/>
     </row>
-    <row r="13" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="18" t="s">
         <v>24</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B14" s="21" t="s">
         <v>25</v>
       </c>
@@ -1040,19 +1040,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="25" t="s">
         <v>33</v>
       </c>
@@ -1066,14 +1066,14 @@
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
     </row>
-    <row r="18" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B18" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="26" t="s">
         <v>34</v>
       </c>
@@ -1096,14 +1096,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B19" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="28" t="s">
         <v>48</v>
       </c>
       <c r="J19" s="3" t="s">

</xml_diff>